<commit_message>
Cambiar valores de la columna Resultados
</commit_message>
<xml_diff>
--- a/OutputFiles/AGOSTO 2025 v2.xlsx
+++ b/OutputFiles/AGOSTO 2025 v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jtccomco-my.sharepoint.com/personal/alan_bohorquez_jtc_com_co/Documents/Escritorio/Alan/Python Projects/OutputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_4B09A086555AD629B52465F1465ED87656CA4840" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E8D99C-3BD2-4E94-9003-B91DC8107E96}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_20A9E29E553A5362318764F1465ED87656CA3051" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D60E90B-045F-483F-B85C-87837114CD77}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
     <t>Contacto No Vinculado A Proveedor</t>
   </si>
   <si>
-    <t>No Encontrado</t>
+    <t>No encontró información</t>
   </si>
   <si>
     <t>9012342823</t>
@@ -163,7 +163,7 @@
     <t>Relación Comercial</t>
   </si>
   <si>
-    <t>Encontrado</t>
+    <t>Entrega Exitosa</t>
   </si>
   <si>
     <t>https://pdf-base64-to-url.onrender.com/public/pdf-1754058459585.pdf</t>
@@ -2617,11 +2617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L648"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A390" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2632,7 +2631,7 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="7" width="35" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="200" customWidth="1"/>
     <col min="11" max="11" width="453" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
@@ -2676,7 +2675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2706,7 +2705,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2736,7 +2735,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2766,7 +2765,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2796,7 +2795,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2826,7 +2825,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2856,7 +2855,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2886,7 +2885,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2916,7 +2915,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -2946,7 +2945,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2976,7 +2975,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3006,7 +3005,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -3036,7 +3035,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -3066,7 +3065,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -3096,7 +3095,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -3126,7 +3125,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -3156,7 +3155,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -3186,7 +3185,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -3218,7 +3217,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -3250,7 +3249,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
@@ -3282,7 +3281,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -3314,7 +3313,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -3346,7 +3345,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -3378,7 +3377,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
@@ -3410,7 +3409,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -3442,7 +3441,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -3474,7 +3473,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -3506,7 +3505,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -3538,7 +3537,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -3642,7 +3641,7 @@
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
@@ -3672,7 +3671,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
@@ -3702,7 +3701,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
@@ -3732,7 +3731,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -3762,7 +3761,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
@@ -3794,7 +3793,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -3826,7 +3825,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -3858,7 +3857,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
@@ -3890,7 +3889,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -3922,7 +3921,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
@@ -3954,7 +3953,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>12</v>
       </c>
@@ -3986,7 +3985,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -4018,7 +4017,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
@@ -4050,7 +4049,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
@@ -4082,7 +4081,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
@@ -4114,7 +4113,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -4146,7 +4145,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>34</v>
       </c>
@@ -4214,7 +4213,7 @@
       </c>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>34</v>
       </c>
@@ -4282,7 +4281,7 @@
       </c>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
@@ -4350,7 +4349,7 @@
       </c>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>12</v>
       </c>
@@ -4378,7 +4377,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>12</v>
       </c>
@@ -4444,7 +4443,7 @@
       </c>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>12</v>
       </c>
@@ -4474,7 +4473,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>12</v>
       </c>
@@ -4504,7 +4503,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>12</v>
       </c>
@@ -4534,7 +4533,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>12</v>
       </c>
@@ -4564,7 +4563,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>12</v>
       </c>
@@ -4594,7 +4593,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>12</v>
       </c>
@@ -4624,7 +4623,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>34</v>
       </c>
@@ -4656,7 +4655,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -4688,7 +4687,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>34</v>
       </c>
@@ -4720,7 +4719,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>34</v>
       </c>
@@ -4752,7 +4751,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>34</v>
       </c>
@@ -4784,7 +4783,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>34</v>
       </c>
@@ -5360,7 +5359,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>103</v>
       </c>
@@ -5390,7 +5389,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>12</v>
       </c>
@@ -5420,7 +5419,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>12</v>
       </c>
@@ -5450,7 +5449,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>12</v>
       </c>
@@ -5480,7 +5479,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>12</v>
       </c>
@@ -5726,7 +5725,7 @@
       </c>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>12</v>
       </c>
@@ -5900,7 +5899,7 @@
       </c>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>32</v>
       </c>
@@ -5932,7 +5931,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>32</v>
       </c>
@@ -5964,7 +5963,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>32</v>
       </c>
@@ -5996,7 +5995,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>32</v>
       </c>
@@ -6028,7 +6027,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>130</v>
       </c>
@@ -6058,7 +6057,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>132</v>
       </c>
@@ -6088,7 +6087,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>12</v>
       </c>
@@ -6118,7 +6117,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>12</v>
       </c>
@@ -6148,7 +6147,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>138</v>
       </c>
@@ -6178,7 +6177,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>138</v>
       </c>
@@ -6928,7 +6927,7 @@
       </c>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>32</v>
       </c>
@@ -6958,7 +6957,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>32</v>
       </c>
@@ -6988,7 +6987,7 @@
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
     </row>
-    <row r="134" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>32</v>
       </c>
@@ -7020,7 +7019,7 @@
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
     </row>
-    <row r="135" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>32</v>
       </c>
@@ -7052,7 +7051,7 @@
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
     </row>
-    <row r="136" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>32</v>
       </c>
@@ -7084,7 +7083,7 @@
       <c r="K136" s="2"/>
       <c r="L136" s="2"/>
     </row>
-    <row r="137" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>32</v>
       </c>
@@ -7116,7 +7115,7 @@
       <c r="K137" s="2"/>
       <c r="L137" s="2"/>
     </row>
-    <row r="138" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>32</v>
       </c>
@@ -7146,7 +7145,7 @@
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
     </row>
-    <row r="139" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>32</v>
       </c>
@@ -7680,7 +7679,7 @@
       </c>
       <c r="L153" s="2"/>
     </row>
-    <row r="154" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>130</v>
       </c>
@@ -7710,7 +7709,7 @@
       <c r="K154" s="2"/>
       <c r="L154" s="2"/>
     </row>
-    <row r="155" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>130</v>
       </c>
@@ -7740,7 +7739,7 @@
       <c r="K155" s="2"/>
       <c r="L155" s="2"/>
     </row>
-    <row r="156" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>130</v>
       </c>
@@ -7770,7 +7769,7 @@
       <c r="K156" s="2"/>
       <c r="L156" s="2"/>
     </row>
-    <row r="157" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>130</v>
       </c>
@@ -7800,7 +7799,7 @@
       <c r="K157" s="2"/>
       <c r="L157" s="2"/>
     </row>
-    <row r="158" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>34</v>
       </c>
@@ -7830,7 +7829,7 @@
       <c r="K158" s="2"/>
       <c r="L158" s="2"/>
     </row>
-    <row r="159" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>34</v>
       </c>
@@ -7860,7 +7859,7 @@
       <c r="K159" s="2"/>
       <c r="L159" s="2"/>
     </row>
-    <row r="160" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>34</v>
       </c>
@@ -7890,7 +7889,7 @@
       <c r="K160" s="2"/>
       <c r="L160" s="2"/>
     </row>
-    <row r="161" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>34</v>
       </c>
@@ -7920,7 +7919,7 @@
       <c r="K161" s="2"/>
       <c r="L161" s="2"/>
     </row>
-    <row r="162" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>152</v>
       </c>
@@ -7950,7 +7949,7 @@
       <c r="K162" s="2"/>
       <c r="L162" s="2"/>
     </row>
-    <row r="163" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>152</v>
       </c>
@@ -7980,7 +7979,7 @@
       <c r="K163" s="2"/>
       <c r="L163" s="2"/>
     </row>
-    <row r="164" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>152</v>
       </c>
@@ -8010,7 +8009,7 @@
       <c r="K164" s="2"/>
       <c r="L164" s="2"/>
     </row>
-    <row r="165" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>152</v>
       </c>
@@ -8040,7 +8039,7 @@
       <c r="K165" s="2"/>
       <c r="L165" s="2"/>
     </row>
-    <row r="166" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>130</v>
       </c>
@@ -8070,7 +8069,7 @@
       <c r="K166" s="2"/>
       <c r="L166" s="2"/>
     </row>
-    <row r="167" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>130</v>
       </c>
@@ -8100,7 +8099,7 @@
       <c r="K167" s="2"/>
       <c r="L167" s="2"/>
     </row>
-    <row r="168" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>130</v>
       </c>
@@ -8130,7 +8129,7 @@
       <c r="K168" s="2"/>
       <c r="L168" s="2"/>
     </row>
-    <row r="169" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>130</v>
       </c>
@@ -8160,7 +8159,7 @@
       <c r="K169" s="2"/>
       <c r="L169" s="2"/>
     </row>
-    <row r="170" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>130</v>
       </c>
@@ -8190,7 +8189,7 @@
       <c r="K170" s="2"/>
       <c r="L170" s="2"/>
     </row>
-    <row r="171" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>198</v>
       </c>
@@ -8220,7 +8219,7 @@
       <c r="K171" s="2"/>
       <c r="L171" s="2"/>
     </row>
-    <row r="172" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>198</v>
       </c>
@@ -8250,7 +8249,7 @@
       <c r="K172" s="2"/>
       <c r="L172" s="2"/>
     </row>
-    <row r="173" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>198</v>
       </c>
@@ -8280,7 +8279,7 @@
       <c r="K173" s="2"/>
       <c r="L173" s="2"/>
     </row>
-    <row r="174" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>198</v>
       </c>
@@ -8310,7 +8309,7 @@
       <c r="K174" s="2"/>
       <c r="L174" s="2"/>
     </row>
-    <row r="175" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>198</v>
       </c>
@@ -8340,7 +8339,7 @@
       <c r="K175" s="2"/>
       <c r="L175" s="2"/>
     </row>
-    <row r="176" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>200</v>
       </c>
@@ -8372,7 +8371,7 @@
       <c r="K176" s="2"/>
       <c r="L176" s="2"/>
     </row>
-    <row r="177" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>200</v>
       </c>
@@ -8404,7 +8403,7 @@
       <c r="K177" s="2"/>
       <c r="L177" s="2"/>
     </row>
-    <row r="178" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>200</v>
       </c>
@@ -8436,7 +8435,7 @@
       <c r="K178" s="2"/>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>200</v>
       </c>
@@ -8504,7 +8503,7 @@
       </c>
       <c r="L180" s="2"/>
     </row>
-    <row r="181" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>200</v>
       </c>
@@ -8536,7 +8535,7 @@
       <c r="K181" s="2"/>
       <c r="L181" s="2"/>
     </row>
-    <row r="182" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>200</v>
       </c>
@@ -8568,7 +8567,7 @@
       <c r="K182" s="2"/>
       <c r="L182" s="2"/>
     </row>
-    <row r="183" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>200</v>
       </c>
@@ -8600,7 +8599,7 @@
       <c r="K183" s="2"/>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>200</v>
       </c>
@@ -8668,7 +8667,7 @@
       </c>
       <c r="L185" s="2"/>
     </row>
-    <row r="186" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>200</v>
       </c>
@@ -8700,7 +8699,7 @@
       <c r="K186" s="2"/>
       <c r="L186" s="2"/>
     </row>
-    <row r="187" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>200</v>
       </c>
@@ -8732,7 +8731,7 @@
       <c r="K187" s="2"/>
       <c r="L187" s="2"/>
     </row>
-    <row r="188" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>200</v>
       </c>
@@ -8764,7 +8763,7 @@
       <c r="K188" s="2"/>
       <c r="L188" s="2"/>
     </row>
-    <row r="189" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>200</v>
       </c>
@@ -8832,7 +8831,7 @@
       </c>
       <c r="L190" s="2"/>
     </row>
-    <row r="191" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>200</v>
       </c>
@@ -8864,7 +8863,7 @@
       <c r="K191" s="2"/>
       <c r="L191" s="2"/>
     </row>
-    <row r="192" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>200</v>
       </c>
@@ -8896,7 +8895,7 @@
       <c r="K192" s="2"/>
       <c r="L192" s="2"/>
     </row>
-    <row r="193" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>200</v>
       </c>
@@ -8928,7 +8927,7 @@
       <c r="K193" s="2"/>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>200</v>
       </c>
@@ -8996,7 +8995,7 @@
       </c>
       <c r="L195" s="2"/>
     </row>
-    <row r="196" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>200</v>
       </c>
@@ -9028,7 +9027,7 @@
       <c r="K196" s="2"/>
       <c r="L196" s="2"/>
     </row>
-    <row r="197" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>200</v>
       </c>
@@ -9060,7 +9059,7 @@
       <c r="K197" s="2"/>
       <c r="L197" s="2"/>
     </row>
-    <row r="198" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>200</v>
       </c>
@@ -9092,7 +9091,7 @@
       <c r="K198" s="2"/>
       <c r="L198" s="2"/>
     </row>
-    <row r="199" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>200</v>
       </c>
@@ -9160,7 +9159,7 @@
       </c>
       <c r="L200" s="2"/>
     </row>
-    <row r="201" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>130</v>
       </c>
@@ -9190,7 +9189,7 @@
       <c r="K201" s="2"/>
       <c r="L201" s="2"/>
     </row>
-    <row r="202" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>130</v>
       </c>
@@ -9220,7 +9219,7 @@
       <c r="K202" s="2"/>
       <c r="L202" s="2"/>
     </row>
-    <row r="203" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>130</v>
       </c>
@@ -9282,7 +9281,7 @@
       <c r="K204" s="2"/>
       <c r="L204" s="2"/>
     </row>
-    <row r="205" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>130</v>
       </c>
@@ -9312,7 +9311,7 @@
       <c r="K205" s="2"/>
       <c r="L205" s="2"/>
     </row>
-    <row r="206" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>198</v>
       </c>
@@ -9340,7 +9339,7 @@
       <c r="K206" s="2"/>
       <c r="L206" s="2"/>
     </row>
-    <row r="207" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>198</v>
       </c>
@@ -9368,7 +9367,7 @@
       <c r="K207" s="2"/>
       <c r="L207" s="2"/>
     </row>
-    <row r="208" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>198</v>
       </c>
@@ -9398,7 +9397,7 @@
       <c r="K208" s="2"/>
       <c r="L208" s="2"/>
     </row>
-    <row r="209" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>198</v>
       </c>
@@ -9428,7 +9427,7 @@
       <c r="K209" s="2"/>
       <c r="L209" s="2"/>
     </row>
-    <row r="210" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>198</v>
       </c>
@@ -9458,7 +9457,7 @@
       <c r="K210" s="2"/>
       <c r="L210" s="2"/>
     </row>
-    <row r="211" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>198</v>
       </c>
@@ -9832,7 +9831,7 @@
       </c>
       <c r="L221" s="2"/>
     </row>
-    <row r="222" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>198</v>
       </c>
@@ -9860,7 +9859,7 @@
       <c r="K222" s="2"/>
       <c r="L222" s="2"/>
     </row>
-    <row r="223" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>198</v>
       </c>
@@ -9962,7 +9961,7 @@
       </c>
       <c r="L225" s="2"/>
     </row>
-    <row r="226" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>198</v>
       </c>
@@ -9992,7 +9991,7 @@
       <c r="K226" s="2"/>
       <c r="L226" s="2"/>
     </row>
-    <row r="227" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>262</v>
       </c>
@@ -10022,7 +10021,7 @@
       <c r="K227" s="2"/>
       <c r="L227" s="2"/>
     </row>
-    <row r="228" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>262</v>
       </c>
@@ -10052,7 +10051,7 @@
       <c r="K228" s="2"/>
       <c r="L228" s="2"/>
     </row>
-    <row r="229" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>262</v>
       </c>
@@ -10222,7 +10221,7 @@
       </c>
       <c r="L233" s="2"/>
     </row>
-    <row r="234" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>34</v>
       </c>
@@ -10254,7 +10253,7 @@
       <c r="K234" s="2"/>
       <c r="L234" s="2"/>
     </row>
-    <row r="235" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>34</v>
       </c>
@@ -10394,7 +10393,7 @@
       </c>
       <c r="L238" s="2"/>
     </row>
-    <row r="239" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>34</v>
       </c>
@@ -10426,7 +10425,7 @@
       <c r="K239" s="2"/>
       <c r="L239" s="2"/>
     </row>
-    <row r="240" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>34</v>
       </c>
@@ -10494,7 +10493,7 @@
       </c>
       <c r="L241" s="2"/>
     </row>
-    <row r="242" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>200</v>
       </c>
@@ -10562,7 +10561,7 @@
       </c>
       <c r="L243" s="2"/>
     </row>
-    <row r="244" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>200</v>
       </c>
@@ -10630,7 +10629,7 @@
       </c>
       <c r="L245" s="2"/>
     </row>
-    <row r="246" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>200</v>
       </c>
@@ -10986,7 +10985,7 @@
       </c>
       <c r="L255" s="2"/>
     </row>
-    <row r="256" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>200</v>
       </c>
@@ -11018,7 +11017,7 @@
       <c r="K256" s="2"/>
       <c r="L256" s="2"/>
     </row>
-    <row r="257" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>200</v>
       </c>
@@ -11086,7 +11085,7 @@
       </c>
       <c r="L258" s="2"/>
     </row>
-    <row r="259" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>200</v>
       </c>
@@ -11154,7 +11153,7 @@
       </c>
       <c r="L260" s="2"/>
     </row>
-    <row r="261" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>200</v>
       </c>
@@ -11222,7 +11221,7 @@
       </c>
       <c r="L262" s="2"/>
     </row>
-    <row r="263" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>200</v>
       </c>
@@ -11578,7 +11577,7 @@
       </c>
       <c r="L272" s="2"/>
     </row>
-    <row r="273" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>200</v>
       </c>
@@ -11610,7 +11609,7 @@
       <c r="K273" s="2"/>
       <c r="L273" s="2"/>
     </row>
-    <row r="274" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>34</v>
       </c>
@@ -11642,7 +11641,7 @@
       <c r="K274" s="2"/>
       <c r="L274" s="2"/>
     </row>
-    <row r="275" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>34</v>
       </c>
@@ -11674,7 +11673,7 @@
       <c r="K275" s="2"/>
       <c r="L275" s="2"/>
     </row>
-    <row r="276" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>34</v>
       </c>
@@ -11706,7 +11705,7 @@
       <c r="K276" s="2"/>
       <c r="L276" s="2"/>
     </row>
-    <row r="277" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>34</v>
       </c>
@@ -11738,7 +11737,7 @@
       <c r="K277" s="2"/>
       <c r="L277" s="2"/>
     </row>
-    <row r="278" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>34</v>
       </c>
@@ -11770,7 +11769,7 @@
       <c r="K278" s="2"/>
       <c r="L278" s="2"/>
     </row>
-    <row r="279" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>34</v>
       </c>
@@ -11802,7 +11801,7 @@
       <c r="K279" s="2"/>
       <c r="L279" s="2"/>
     </row>
-    <row r="280" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>34</v>
       </c>
@@ -11834,7 +11833,7 @@
       <c r="K280" s="2"/>
       <c r="L280" s="2"/>
     </row>
-    <row r="281" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>34</v>
       </c>
@@ -11866,7 +11865,7 @@
       <c r="K281" s="2"/>
       <c r="L281" s="2"/>
     </row>
-    <row r="282" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>34</v>
       </c>
@@ -11898,7 +11897,7 @@
       <c r="K282" s="2"/>
       <c r="L282" s="2"/>
     </row>
-    <row r="283" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>34</v>
       </c>
@@ -11930,7 +11929,7 @@
       <c r="K283" s="2"/>
       <c r="L283" s="2"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>34</v>
       </c>
@@ -11960,7 +11959,7 @@
       <c r="K284" s="2"/>
       <c r="L284" s="2"/>
     </row>
-    <row r="285" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>34</v>
       </c>
@@ -11988,7 +11987,7 @@
       <c r="K285" s="2"/>
       <c r="L285" s="2"/>
     </row>
-    <row r="286" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>146</v>
       </c>
@@ -12018,7 +12017,7 @@
       <c r="K286" s="2"/>
       <c r="L286" s="2"/>
     </row>
-    <row r="287" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>146</v>
       </c>
@@ -12084,7 +12083,7 @@
       </c>
       <c r="L288" s="2"/>
     </row>
-    <row r="289" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>313</v>
       </c>
@@ -12150,7 +12149,7 @@
       </c>
       <c r="L290" s="2"/>
     </row>
-    <row r="291" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>34</v>
       </c>
@@ -12612,7 +12611,7 @@
       </c>
       <c r="L303" s="2"/>
     </row>
-    <row r="304" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>97</v>
       </c>
@@ -12644,7 +12643,7 @@
       <c r="K304" s="2"/>
       <c r="L304" s="2"/>
     </row>
-    <row r="305" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>97</v>
       </c>
@@ -12676,7 +12675,7 @@
       <c r="K305" s="2"/>
       <c r="L305" s="2"/>
     </row>
-    <row r="306" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>97</v>
       </c>
@@ -12708,7 +12707,7 @@
       <c r="K306" s="2"/>
       <c r="L306" s="2"/>
     </row>
-    <row r="307" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>97</v>
       </c>
@@ -12740,7 +12739,7 @@
       <c r="K307" s="2"/>
       <c r="L307" s="2"/>
     </row>
-    <row r="308" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>97</v>
       </c>
@@ -12772,7 +12771,7 @@
       <c r="K308" s="2"/>
       <c r="L308" s="2"/>
     </row>
-    <row r="309" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>97</v>
       </c>
@@ -12804,7 +12803,7 @@
       <c r="K309" s="2"/>
       <c r="L309" s="2"/>
     </row>
-    <row r="310" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>97</v>
       </c>
@@ -12836,7 +12835,7 @@
       <c r="K310" s="2"/>
       <c r="L310" s="2"/>
     </row>
-    <row r="311" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>97</v>
       </c>
@@ -12868,7 +12867,7 @@
       <c r="K311" s="2"/>
       <c r="L311" s="2"/>
     </row>
-    <row r="312" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>97</v>
       </c>
@@ -12900,7 +12899,7 @@
       <c r="K312" s="2"/>
       <c r="L312" s="2"/>
     </row>
-    <row r="313" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>97</v>
       </c>
@@ -12932,7 +12931,7 @@
       <c r="K313" s="2"/>
       <c r="L313" s="2"/>
     </row>
-    <row r="314" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>97</v>
       </c>
@@ -12964,7 +12963,7 @@
       <c r="K314" s="2"/>
       <c r="L314" s="2"/>
     </row>
-    <row r="315" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>97</v>
       </c>
@@ -12996,7 +12995,7 @@
       <c r="K315" s="2"/>
       <c r="L315" s="2"/>
     </row>
-    <row r="316" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>97</v>
       </c>
@@ -13028,7 +13027,7 @@
       <c r="K316" s="2"/>
       <c r="L316" s="2"/>
     </row>
-    <row r="317" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>97</v>
       </c>
@@ -13060,7 +13059,7 @@
       <c r="K317" s="2"/>
       <c r="L317" s="2"/>
     </row>
-    <row r="318" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>97</v>
       </c>
@@ -13092,7 +13091,7 @@
       <c r="K318" s="2"/>
       <c r="L318" s="2"/>
     </row>
-    <row r="319" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>97</v>
       </c>
@@ -13124,7 +13123,7 @@
       <c r="K319" s="2"/>
       <c r="L319" s="2"/>
     </row>
-    <row r="320" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>97</v>
       </c>
@@ -13156,7 +13155,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="2"/>
     </row>
-    <row r="321" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>97</v>
       </c>
@@ -13188,7 +13187,7 @@
       <c r="K321" s="2"/>
       <c r="L321" s="2"/>
     </row>
-    <row r="322" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>97</v>
       </c>
@@ -13220,7 +13219,7 @@
       <c r="K322" s="2"/>
       <c r="L322" s="2"/>
     </row>
-    <row r="323" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>97</v>
       </c>
@@ -13252,7 +13251,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="2"/>
     </row>
-    <row r="324" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>97</v>
       </c>
@@ -13284,7 +13283,7 @@
       <c r="K324" s="2"/>
       <c r="L324" s="2"/>
     </row>
-    <row r="325" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>97</v>
       </c>
@@ -13316,7 +13315,7 @@
       <c r="K325" s="2"/>
       <c r="L325" s="2"/>
     </row>
-    <row r="326" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>97</v>
       </c>
@@ -13348,7 +13347,7 @@
       <c r="K326" s="2"/>
       <c r="L326" s="2"/>
     </row>
-    <row r="327" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>97</v>
       </c>
@@ -13380,7 +13379,7 @@
       <c r="K327" s="2"/>
       <c r="L327" s="2"/>
     </row>
-    <row r="328" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>343</v>
       </c>
@@ -13412,7 +13411,7 @@
       <c r="K328" s="2"/>
       <c r="L328" s="2"/>
     </row>
-    <row r="329" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>343</v>
       </c>
@@ -13444,7 +13443,7 @@
       <c r="K329" s="2"/>
       <c r="L329" s="2"/>
     </row>
-    <row r="330" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>343</v>
       </c>
@@ -13476,7 +13475,7 @@
       <c r="K330" s="2"/>
       <c r="L330" s="2"/>
     </row>
-    <row r="331" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>343</v>
       </c>
@@ -13508,7 +13507,7 @@
       <c r="K331" s="2"/>
       <c r="L331" s="2"/>
     </row>
-    <row r="332" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>343</v>
       </c>
@@ -13540,7 +13539,7 @@
       <c r="K332" s="2"/>
       <c r="L332" s="2"/>
     </row>
-    <row r="333" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>343</v>
       </c>
@@ -13572,7 +13571,7 @@
       <c r="K333" s="2"/>
       <c r="L333" s="2"/>
     </row>
-    <row r="334" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>343</v>
       </c>
@@ -13604,7 +13603,7 @@
       <c r="K334" s="2"/>
       <c r="L334" s="2"/>
     </row>
-    <row r="335" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>343</v>
       </c>
@@ -13636,7 +13635,7 @@
       <c r="K335" s="2"/>
       <c r="L335" s="2"/>
     </row>
-    <row r="336" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>343</v>
       </c>
@@ -13668,7 +13667,7 @@
       <c r="K336" s="2"/>
       <c r="L336" s="2"/>
     </row>
-    <row r="337" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>343</v>
       </c>
@@ -13700,7 +13699,7 @@
       <c r="K337" s="2"/>
       <c r="L337" s="2"/>
     </row>
-    <row r="338" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>343</v>
       </c>
@@ -13732,7 +13731,7 @@
       <c r="K338" s="2"/>
       <c r="L338" s="2"/>
     </row>
-    <row r="339" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>343</v>
       </c>
@@ -13764,7 +13763,7 @@
       <c r="K339" s="2"/>
       <c r="L339" s="2"/>
     </row>
-    <row r="340" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>345</v>
       </c>
@@ -13832,7 +13831,7 @@
       </c>
       <c r="L341" s="2"/>
     </row>
-    <row r="342" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>345</v>
       </c>
@@ -13900,7 +13899,7 @@
       </c>
       <c r="L343" s="2"/>
     </row>
-    <row r="344" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>345</v>
       </c>
@@ -13968,7 +13967,7 @@
       </c>
       <c r="L345" s="2"/>
     </row>
-    <row r="346" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>345</v>
       </c>
@@ -14036,7 +14035,7 @@
       </c>
       <c r="L347" s="2"/>
     </row>
-    <row r="348" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>345</v>
       </c>
@@ -14104,7 +14103,7 @@
       </c>
       <c r="L349" s="2"/>
     </row>
-    <row r="350" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>345</v>
       </c>
@@ -14172,7 +14171,7 @@
       </c>
       <c r="L351" s="2"/>
     </row>
-    <row r="352" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>34</v>
       </c>
@@ -14202,7 +14201,7 @@
       <c r="K352" s="2"/>
       <c r="L352" s="2"/>
     </row>
-    <row r="353" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>34</v>
       </c>
@@ -14808,7 +14807,7 @@
       </c>
       <c r="L369" s="2"/>
     </row>
-    <row r="370" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>34</v>
       </c>
@@ -14838,7 +14837,7 @@
       <c r="K370" s="2"/>
       <c r="L370" s="2"/>
     </row>
-    <row r="371" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>34</v>
       </c>
@@ -14868,7 +14867,7 @@
       <c r="K371" s="2"/>
       <c r="L371" s="2"/>
     </row>
-    <row r="372" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>34</v>
       </c>
@@ -14900,7 +14899,7 @@
       <c r="K372" s="2"/>
       <c r="L372" s="2"/>
     </row>
-    <row r="373" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>34</v>
       </c>
@@ -14932,7 +14931,7 @@
       <c r="K373" s="2"/>
       <c r="L373" s="2"/>
     </row>
-    <row r="374" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>34</v>
       </c>
@@ -14964,7 +14963,7 @@
       <c r="K374" s="2"/>
       <c r="L374" s="2"/>
     </row>
-    <row r="375" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>116</v>
       </c>
@@ -14996,7 +14995,7 @@
       <c r="K375" s="2"/>
       <c r="L375" s="2"/>
     </row>
-    <row r="376" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>116</v>
       </c>
@@ -15028,7 +15027,7 @@
       <c r="K376" s="2"/>
       <c r="L376" s="2"/>
     </row>
-    <row r="377" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>116</v>
       </c>
@@ -15132,7 +15131,7 @@
       </c>
       <c r="L379" s="2"/>
     </row>
-    <row r="380" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>152</v>
       </c>
@@ -15236,7 +15235,7 @@
       </c>
       <c r="L382" s="2"/>
     </row>
-    <row r="383" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>152</v>
       </c>
@@ -15340,7 +15339,7 @@
       </c>
       <c r="L385" s="2"/>
     </row>
-    <row r="386" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>152</v>
       </c>
@@ -15372,7 +15371,7 @@
       <c r="K386" s="2"/>
       <c r="L386" s="2"/>
     </row>
-    <row r="387" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>34</v>
       </c>
@@ -15402,7 +15401,7 @@
       <c r="K387" s="2"/>
       <c r="L387" s="2"/>
     </row>
-    <row r="388" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>34</v>
       </c>
@@ -15432,7 +15431,7 @@
       <c r="K388" s="2"/>
       <c r="L388" s="2"/>
     </row>
-    <row r="389" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>34</v>
       </c>
@@ -15536,7 +15535,7 @@
       </c>
       <c r="L391" s="2"/>
     </row>
-    <row r="392" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>34</v>
       </c>
@@ -15640,7 +15639,7 @@
       </c>
       <c r="L394" s="2"/>
     </row>
-    <row r="395" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>34</v>
       </c>
@@ -15672,7 +15671,7 @@
       <c r="K395" s="2"/>
       <c r="L395" s="2"/>
     </row>
-    <row r="396" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>34</v>
       </c>
@@ -15704,7 +15703,7 @@
       <c r="K396" s="2"/>
       <c r="L396" s="2"/>
     </row>
-    <row r="397" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>34</v>
       </c>
@@ -15736,7 +15735,7 @@
       <c r="K397" s="2"/>
       <c r="L397" s="2"/>
     </row>
-    <row r="398" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>34</v>
       </c>
@@ -15840,7 +15839,7 @@
       </c>
       <c r="L400" s="2"/>
     </row>
-    <row r="401" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>34</v>
       </c>
@@ -15944,7 +15943,7 @@
       </c>
       <c r="L403" s="2"/>
     </row>
-    <row r="404" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
         <v>34</v>
       </c>
@@ -15976,7 +15975,7 @@
       <c r="K404" s="2"/>
       <c r="L404" s="2"/>
     </row>
-    <row r="405" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>34</v>
       </c>
@@ -16008,7 +16007,7 @@
       <c r="K405" s="2"/>
       <c r="L405" s="2"/>
     </row>
-    <row r="406" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>34</v>
       </c>
@@ -16040,7 +16039,7 @@
       <c r="K406" s="2"/>
       <c r="L406" s="2"/>
     </row>
-    <row r="407" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>34</v>
       </c>
@@ -16144,7 +16143,7 @@
       </c>
       <c r="L409" s="2"/>
     </row>
-    <row r="410" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
         <v>34</v>
       </c>
@@ -16248,7 +16247,7 @@
       </c>
       <c r="L412" s="2"/>
     </row>
-    <row r="413" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>34</v>
       </c>
@@ -16280,7 +16279,7 @@
       <c r="K413" s="2"/>
       <c r="L413" s="2"/>
     </row>
-    <row r="414" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
         <v>34</v>
       </c>
@@ -16312,7 +16311,7 @@
       <c r="K414" s="2"/>
       <c r="L414" s="2"/>
     </row>
-    <row r="415" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>34</v>
       </c>
@@ -16488,7 +16487,7 @@
       </c>
       <c r="L419" s="2"/>
     </row>
-    <row r="420" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
         <v>343</v>
       </c>
@@ -16556,7 +16555,7 @@
       </c>
       <c r="L421" s="2"/>
     </row>
-    <row r="422" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>343</v>
       </c>
@@ -16588,7 +16587,7 @@
       <c r="K422" s="2"/>
       <c r="L422" s="2"/>
     </row>
-    <row r="423" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>343</v>
       </c>
@@ -16620,7 +16619,7 @@
       <c r="K423" s="2"/>
       <c r="L423" s="2"/>
     </row>
-    <row r="424" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>343</v>
       </c>
@@ -16724,7 +16723,7 @@
       </c>
       <c r="L426" s="2"/>
     </row>
-    <row r="427" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>343</v>
       </c>
@@ -16756,7 +16755,7 @@
       <c r="K427" s="2"/>
       <c r="L427" s="2"/>
     </row>
-    <row r="428" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>343</v>
       </c>
@@ -16788,7 +16787,7 @@
       <c r="K428" s="2"/>
       <c r="L428" s="2"/>
     </row>
-    <row r="429" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>343</v>
       </c>
@@ -16820,7 +16819,7 @@
       <c r="K429" s="2"/>
       <c r="L429" s="2"/>
     </row>
-    <row r="430" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
         <v>343</v>
       </c>
@@ -16852,7 +16851,7 @@
       <c r="K430" s="2"/>
       <c r="L430" s="2"/>
     </row>
-    <row r="431" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>343</v>
       </c>
@@ -16884,7 +16883,7 @@
       <c r="K431" s="2"/>
       <c r="L431" s="2"/>
     </row>
-    <row r="432" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
         <v>343</v>
       </c>
@@ -17060,7 +17059,7 @@
       </c>
       <c r="L436" s="2"/>
     </row>
-    <row r="437" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
         <v>343</v>
       </c>
@@ -17128,7 +17127,7 @@
       </c>
       <c r="L438" s="2"/>
     </row>
-    <row r="439" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
         <v>343</v>
       </c>
@@ -17160,7 +17159,7 @@
       <c r="K439" s="2"/>
       <c r="L439" s="2"/>
     </row>
-    <row r="440" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
         <v>343</v>
       </c>
@@ -17192,7 +17191,7 @@
       <c r="K440" s="2"/>
       <c r="L440" s="2"/>
     </row>
-    <row r="441" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
         <v>343</v>
       </c>
@@ -17296,7 +17295,7 @@
       </c>
       <c r="L443" s="2"/>
     </row>
-    <row r="444" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
         <v>343</v>
       </c>
@@ -17328,7 +17327,7 @@
       <c r="K444" s="2"/>
       <c r="L444" s="2"/>
     </row>
-    <row r="445" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>343</v>
       </c>
@@ -17360,7 +17359,7 @@
       <c r="K445" s="2"/>
       <c r="L445" s="2"/>
     </row>
-    <row r="446" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>343</v>
       </c>
@@ -17392,7 +17391,7 @@
       <c r="K446" s="2"/>
       <c r="L446" s="2"/>
     </row>
-    <row r="447" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
         <v>343</v>
       </c>
@@ -17424,7 +17423,7 @@
       <c r="K447" s="2"/>
       <c r="L447" s="2"/>
     </row>
-    <row r="448" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
         <v>343</v>
       </c>
@@ -17456,7 +17455,7 @@
       <c r="K448" s="2"/>
       <c r="L448" s="2"/>
     </row>
-    <row r="449" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
         <v>343</v>
       </c>
@@ -17632,7 +17631,7 @@
       </c>
       <c r="L453" s="2"/>
     </row>
-    <row r="454" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>343</v>
       </c>
@@ -17700,7 +17699,7 @@
       </c>
       <c r="L455" s="2"/>
     </row>
-    <row r="456" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>343</v>
       </c>
@@ -17732,7 +17731,7 @@
       <c r="K456" s="2"/>
       <c r="L456" s="2"/>
     </row>
-    <row r="457" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>343</v>
       </c>
@@ -17764,7 +17763,7 @@
       <c r="K457" s="2"/>
       <c r="L457" s="2"/>
     </row>
-    <row r="458" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
         <v>343</v>
       </c>
@@ -17868,7 +17867,7 @@
       </c>
       <c r="L460" s="2"/>
     </row>
-    <row r="461" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>343</v>
       </c>
@@ -17900,7 +17899,7 @@
       <c r="K461" s="2"/>
       <c r="L461" s="2"/>
     </row>
-    <row r="462" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>343</v>
       </c>
@@ -17932,7 +17931,7 @@
       <c r="K462" s="2"/>
       <c r="L462" s="2"/>
     </row>
-    <row r="463" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>343</v>
       </c>
@@ -17964,7 +17963,7 @@
       <c r="K463" s="2"/>
       <c r="L463" s="2"/>
     </row>
-    <row r="464" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
         <v>343</v>
       </c>
@@ -17996,7 +17995,7 @@
       <c r="K464" s="2"/>
       <c r="L464" s="2"/>
     </row>
-    <row r="465" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>343</v>
       </c>
@@ -18028,7 +18027,7 @@
       <c r="K465" s="2"/>
       <c r="L465" s="2"/>
     </row>
-    <row r="466" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>343</v>
       </c>
@@ -18060,7 +18059,7 @@
       <c r="K466" s="2"/>
       <c r="L466" s="2"/>
     </row>
-    <row r="467" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
         <v>34</v>
       </c>
@@ -18092,7 +18091,7 @@
       <c r="K467" s="2"/>
       <c r="L467" s="2"/>
     </row>
-    <row r="468" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="2" t="s">
         <v>34</v>
       </c>
@@ -18160,7 +18159,7 @@
       </c>
       <c r="L469" s="2"/>
     </row>
-    <row r="470" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="2" t="s">
         <v>34</v>
       </c>
@@ -18192,7 +18191,7 @@
       <c r="K470" s="2"/>
       <c r="L470" s="2"/>
     </row>
-    <row r="471" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
         <v>34</v>
       </c>
@@ -18260,7 +18259,7 @@
       </c>
       <c r="L472" s="2"/>
     </row>
-    <row r="473" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
         <v>97</v>
       </c>
@@ -18328,7 +18327,7 @@
       </c>
       <c r="L474" s="2"/>
     </row>
-    <row r="475" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
         <v>97</v>
       </c>
@@ -18396,7 +18395,7 @@
       </c>
       <c r="L476" s="2"/>
     </row>
-    <row r="477" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
         <v>313</v>
       </c>
@@ -18460,7 +18459,7 @@
       </c>
       <c r="L478" s="2"/>
     </row>
-    <row r="479" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
         <v>429</v>
       </c>
@@ -18588,7 +18587,7 @@
       <c r="K482" s="2"/>
       <c r="L482" s="2"/>
     </row>
-    <row r="483" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
         <v>152</v>
       </c>
@@ -18620,7 +18619,7 @@
       <c r="K483" s="2"/>
       <c r="L483" s="2"/>
     </row>
-    <row r="484" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
         <v>152</v>
       </c>
@@ -18652,7 +18651,7 @@
       <c r="K484" s="2"/>
       <c r="L484" s="2"/>
     </row>
-    <row r="485" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
         <v>200</v>
       </c>
@@ -18684,7 +18683,7 @@
       <c r="K485" s="2"/>
       <c r="L485" s="2"/>
     </row>
-    <row r="486" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" s="2" t="s">
         <v>200</v>
       </c>
@@ -18752,7 +18751,7 @@
       </c>
       <c r="L487" s="2"/>
     </row>
-    <row r="488" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
         <v>200</v>
       </c>
@@ -18782,7 +18781,7 @@
       <c r="K488" s="2"/>
       <c r="L488" s="2"/>
     </row>
-    <row r="489" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
         <v>200</v>
       </c>
@@ -18814,7 +18813,7 @@
       <c r="K489" s="2"/>
       <c r="L489" s="2"/>
     </row>
-    <row r="490" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
         <v>200</v>
       </c>
@@ -18846,7 +18845,7 @@
       <c r="K490" s="2"/>
       <c r="L490" s="2"/>
     </row>
-    <row r="491" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
         <v>200</v>
       </c>
@@ -18878,7 +18877,7 @@
       <c r="K491" s="2"/>
       <c r="L491" s="2"/>
     </row>
-    <row r="492" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
         <v>200</v>
       </c>
@@ -18910,7 +18909,7 @@
       <c r="K492" s="2"/>
       <c r="L492" s="2"/>
     </row>
-    <row r="493" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
         <v>132</v>
       </c>
@@ -18938,7 +18937,7 @@
       <c r="K493" s="2"/>
       <c r="L493" s="2"/>
     </row>
-    <row r="494" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" s="2" t="s">
         <v>132</v>
       </c>
@@ -19324,7 +19323,7 @@
       <c r="K504" s="2"/>
       <c r="L504" s="2"/>
     </row>
-    <row r="505" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
         <v>132</v>
       </c>
@@ -19354,7 +19353,7 @@
       <c r="K505" s="2"/>
       <c r="L505" s="2"/>
     </row>
-    <row r="506" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" s="2" t="s">
         <v>132</v>
       </c>
@@ -19384,7 +19383,7 @@
       <c r="K506" s="2"/>
       <c r="L506" s="2"/>
     </row>
-    <row r="507" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
         <v>132</v>
       </c>
@@ -19414,7 +19413,7 @@
       <c r="K507" s="2"/>
       <c r="L507" s="2"/>
     </row>
-    <row r="508" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" s="2" t="s">
         <v>132</v>
       </c>
@@ -19444,7 +19443,7 @@
       <c r="K508" s="2"/>
       <c r="L508" s="2"/>
     </row>
-    <row r="509" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
         <v>132</v>
       </c>
@@ -19474,7 +19473,7 @@
       <c r="K509" s="2"/>
       <c r="L509" s="2"/>
     </row>
-    <row r="510" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
         <v>132</v>
       </c>
@@ -19504,7 +19503,7 @@
       <c r="K510" s="2"/>
       <c r="L510" s="2"/>
     </row>
-    <row r="511" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
         <v>97</v>
       </c>
@@ -19536,7 +19535,7 @@
       <c r="K511" s="2"/>
       <c r="L511" s="2"/>
     </row>
-    <row r="512" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
         <v>97</v>
       </c>
@@ -19568,7 +19567,7 @@
       <c r="K512" s="2"/>
       <c r="L512" s="2"/>
     </row>
-    <row r="513" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
         <v>97</v>
       </c>
@@ -19600,7 +19599,7 @@
       <c r="K513" s="2"/>
       <c r="L513" s="2"/>
     </row>
-    <row r="514" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" s="2" t="s">
         <v>97</v>
       </c>
@@ -19700,7 +19699,7 @@
       </c>
       <c r="L516" s="2"/>
     </row>
-    <row r="517" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
         <v>146</v>
       </c>
@@ -19768,7 +19767,7 @@
       </c>
       <c r="L518" s="2"/>
     </row>
-    <row r="519" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
         <v>146</v>
       </c>
@@ -19836,7 +19835,7 @@
       </c>
       <c r="L520" s="2"/>
     </row>
-    <row r="521" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" s="2" t="s">
         <v>146</v>
       </c>
@@ -19868,7 +19867,7 @@
       <c r="K521" s="2"/>
       <c r="L521" s="2"/>
     </row>
-    <row r="522" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" s="2" t="s">
         <v>97</v>
       </c>
@@ -19900,7 +19899,7 @@
       <c r="K522" s="2"/>
       <c r="L522" s="2"/>
     </row>
-    <row r="523" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" s="2" t="s">
         <v>97</v>
       </c>
@@ -19932,7 +19931,7 @@
       <c r="K523" s="2"/>
       <c r="L523" s="2"/>
     </row>
-    <row r="524" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" s="2" t="s">
         <v>97</v>
       </c>
@@ -19964,7 +19963,7 @@
       <c r="K524" s="2"/>
       <c r="L524" s="2"/>
     </row>
-    <row r="525" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
         <v>152</v>
       </c>
@@ -19996,7 +19995,7 @@
       <c r="K525" s="2"/>
       <c r="L525" s="2"/>
     </row>
-    <row r="526" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" s="2" t="s">
         <v>152</v>
       </c>
@@ -20028,7 +20027,7 @@
       <c r="K526" s="2"/>
       <c r="L526" s="2"/>
     </row>
-    <row r="527" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527" s="2" t="s">
         <v>152</v>
       </c>
@@ -20092,7 +20091,7 @@
       <c r="K528" s="2"/>
       <c r="L528" s="2"/>
     </row>
-    <row r="529" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529" s="2" t="s">
         <v>152</v>
       </c>
@@ -20124,7 +20123,7 @@
       <c r="K529" s="2"/>
       <c r="L529" s="2"/>
     </row>
-    <row r="530" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" s="2" t="s">
         <v>152</v>
       </c>
@@ -20156,7 +20155,7 @@
       <c r="K530" s="2"/>
       <c r="L530" s="2"/>
     </row>
-    <row r="531" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531" s="2" t="s">
         <v>152</v>
       </c>
@@ -20220,7 +20219,7 @@
       <c r="K532" s="2"/>
       <c r="L532" s="2"/>
     </row>
-    <row r="533" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" s="2" t="s">
         <v>152</v>
       </c>
@@ -20252,7 +20251,7 @@
       <c r="K533" s="2"/>
       <c r="L533" s="2"/>
     </row>
-    <row r="534" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" s="2" t="s">
         <v>152</v>
       </c>
@@ -20284,7 +20283,7 @@
       <c r="K534" s="2"/>
       <c r="L534" s="2"/>
     </row>
-    <row r="535" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
         <v>152</v>
       </c>
@@ -20348,7 +20347,7 @@
       <c r="K536" s="2"/>
       <c r="L536" s="2"/>
     </row>
-    <row r="537" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
         <v>146</v>
       </c>
@@ -20378,7 +20377,7 @@
       <c r="K537" s="2"/>
       <c r="L537" s="2"/>
     </row>
-    <row r="538" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" s="2" t="s">
         <v>146</v>
       </c>
@@ -20406,7 +20405,7 @@
       <c r="K538" s="2"/>
       <c r="L538" s="2"/>
     </row>
-    <row r="539" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
         <v>369</v>
       </c>
@@ -20438,7 +20437,7 @@
       <c r="K539" s="2"/>
       <c r="L539" s="2"/>
     </row>
-    <row r="540" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540" s="2" t="s">
         <v>369</v>
       </c>
@@ -20468,7 +20467,7 @@
       <c r="K540" s="2"/>
       <c r="L540" s="2"/>
     </row>
-    <row r="541" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" s="2" t="s">
         <v>530</v>
       </c>
@@ -20496,7 +20495,7 @@
       <c r="K541" s="2"/>
       <c r="L541" s="2"/>
     </row>
-    <row r="542" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542" s="2" t="s">
         <v>530</v>
       </c>
@@ -20526,7 +20525,7 @@
       <c r="K542" s="2"/>
       <c r="L542" s="2"/>
     </row>
-    <row r="543" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" s="2" t="s">
         <v>530</v>
       </c>
@@ -20554,7 +20553,7 @@
       <c r="K543" s="2"/>
       <c r="L543" s="2"/>
     </row>
-    <row r="544" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" s="2" t="s">
         <v>540</v>
       </c>
@@ -20582,7 +20581,7 @@
       <c r="K544" s="2"/>
       <c r="L544" s="2"/>
     </row>
-    <row r="545" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545" s="2" t="s">
         <v>540</v>
       </c>
@@ -20610,7 +20609,7 @@
       <c r="K545" s="2"/>
       <c r="L545" s="2"/>
     </row>
-    <row r="546" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A546" s="2" t="s">
         <v>547</v>
       </c>
@@ -20638,7 +20637,7 @@
       <c r="K546" s="2"/>
       <c r="L546" s="2"/>
     </row>
-    <row r="547" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" s="2" t="s">
         <v>149</v>
       </c>
@@ -20666,7 +20665,7 @@
       <c r="K547" s="2"/>
       <c r="L547" s="2"/>
     </row>
-    <row r="548" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" s="2" t="s">
         <v>149</v>
       </c>
@@ -20730,7 +20729,7 @@
       <c r="K549" s="2"/>
       <c r="L549" s="2"/>
     </row>
-    <row r="550" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" s="2" t="s">
         <v>149</v>
       </c>
@@ -20760,7 +20759,7 @@
       <c r="K550" s="2"/>
       <c r="L550" s="2"/>
     </row>
-    <row r="551" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" s="2" t="s">
         <v>149</v>
       </c>
@@ -20788,7 +20787,7 @@
       <c r="K551" s="2"/>
       <c r="L551" s="2"/>
     </row>
-    <row r="552" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A552" s="2" t="s">
         <v>345</v>
       </c>
@@ -20816,7 +20815,7 @@
       <c r="K552" s="2"/>
       <c r="L552" s="2"/>
     </row>
-    <row r="553" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" s="2" t="s">
         <v>149</v>
       </c>
@@ -21134,7 +21133,7 @@
       </c>
       <c r="L561" s="2"/>
     </row>
-    <row r="562" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A562" s="2" t="s">
         <v>177</v>
       </c>
@@ -21232,7 +21231,7 @@
       <c r="K564" s="2"/>
       <c r="L564" s="2"/>
     </row>
-    <row r="565" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" s="2" t="s">
         <v>177</v>
       </c>
@@ -21262,7 +21261,7 @@
       <c r="K565" s="2"/>
       <c r="L565" s="2"/>
     </row>
-    <row r="566" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A566" s="2" t="s">
         <v>177</v>
       </c>
@@ -21292,7 +21291,7 @@
       <c r="K566" s="2"/>
       <c r="L566" s="2"/>
     </row>
-    <row r="567" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A567" s="2" t="s">
         <v>177</v>
       </c>
@@ -21322,7 +21321,7 @@
       <c r="K567" s="2"/>
       <c r="L567" s="2"/>
     </row>
-    <row r="568" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A568" s="2" t="s">
         <v>177</v>
       </c>
@@ -21350,7 +21349,7 @@
       <c r="K568" s="2"/>
       <c r="L568" s="2"/>
     </row>
-    <row r="569" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A569" s="2" t="s">
         <v>177</v>
       </c>
@@ -21380,7 +21379,7 @@
       <c r="K569" s="2"/>
       <c r="L569" s="2"/>
     </row>
-    <row r="570" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A570" s="2" t="s">
         <v>97</v>
       </c>
@@ -21408,7 +21407,7 @@
       <c r="K570" s="2"/>
       <c r="L570" s="2"/>
     </row>
-    <row r="571" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571" s="2" t="s">
         <v>97</v>
       </c>
@@ -21436,7 +21435,7 @@
       <c r="K571" s="2"/>
       <c r="L571" s="2"/>
     </row>
-    <row r="572" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A572" s="2" t="s">
         <v>97</v>
       </c>
@@ -21466,7 +21465,7 @@
       <c r="K572" s="2"/>
       <c r="L572" s="2"/>
     </row>
-    <row r="573" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A573" s="2" t="s">
         <v>97</v>
       </c>
@@ -21496,7 +21495,7 @@
       <c r="K573" s="2"/>
       <c r="L573" s="2"/>
     </row>
-    <row r="574" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A574" s="2" t="s">
         <v>97</v>
       </c>
@@ -21524,7 +21523,7 @@
       <c r="K574" s="2"/>
       <c r="L574" s="2"/>
     </row>
-    <row r="575" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A575" s="2" t="s">
         <v>97</v>
       </c>
@@ -21554,7 +21553,7 @@
       <c r="K575" s="2"/>
       <c r="L575" s="2"/>
     </row>
-    <row r="576" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576" s="2" t="s">
         <v>97</v>
       </c>
@@ -21584,7 +21583,7 @@
       <c r="K576" s="2"/>
       <c r="L576" s="2"/>
     </row>
-    <row r="577" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A577" s="2" t="s">
         <v>97</v>
       </c>
@@ -21614,7 +21613,7 @@
       <c r="K577" s="2"/>
       <c r="L577" s="2"/>
     </row>
-    <row r="578" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A578" s="2" t="s">
         <v>97</v>
       </c>
@@ -21644,7 +21643,7 @@
       <c r="K578" s="2"/>
       <c r="L578" s="2"/>
     </row>
-    <row r="579" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A579" s="2" t="s">
         <v>97</v>
       </c>
@@ -21674,7 +21673,7 @@
       <c r="K579" s="2"/>
       <c r="L579" s="2"/>
     </row>
-    <row r="580" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A580" s="2" t="s">
         <v>97</v>
       </c>
@@ -21702,7 +21701,7 @@
       <c r="K580" s="2"/>
       <c r="L580" s="2"/>
     </row>
-    <row r="581" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A581" s="2" t="s">
         <v>116</v>
       </c>
@@ -21770,7 +21769,7 @@
       </c>
       <c r="L582" s="2"/>
     </row>
-    <row r="583" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583" s="2" t="s">
         <v>116</v>
       </c>
@@ -21802,7 +21801,7 @@
       <c r="K583" s="2"/>
       <c r="L583" s="2"/>
     </row>
-    <row r="584" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584" s="2" t="s">
         <v>116</v>
       </c>
@@ -21834,7 +21833,7 @@
       <c r="K584" s="2"/>
       <c r="L584" s="2"/>
     </row>
-    <row r="585" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A585" s="2" t="s">
         <v>116</v>
       </c>
@@ -21938,7 +21937,7 @@
       </c>
       <c r="L587" s="2"/>
     </row>
-    <row r="588" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A588" s="2" t="s">
         <v>116</v>
       </c>
@@ -21970,7 +21969,7 @@
       <c r="K588" s="2"/>
       <c r="L588" s="2"/>
     </row>
-    <row r="589" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A589" s="2" t="s">
         <v>116</v>
       </c>
@@ -22002,7 +22001,7 @@
       <c r="K589" s="2"/>
       <c r="L589" s="2"/>
     </row>
-    <row r="590" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A590" s="2" t="s">
         <v>116</v>
       </c>
@@ -22034,7 +22033,7 @@
       <c r="K590" s="2"/>
       <c r="L590" s="2"/>
     </row>
-    <row r="591" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A591" s="2" t="s">
         <v>116</v>
       </c>
@@ -22066,7 +22065,7 @@
       <c r="K591" s="2"/>
       <c r="L591" s="2"/>
     </row>
-    <row r="592" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A592" s="2" t="s">
         <v>116</v>
       </c>
@@ -22098,7 +22097,7 @@
       <c r="K592" s="2"/>
       <c r="L592" s="2"/>
     </row>
-    <row r="593" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A593" s="2" t="s">
         <v>116</v>
       </c>
@@ -22130,7 +22129,7 @@
       <c r="K593" s="2"/>
       <c r="L593" s="2"/>
     </row>
-    <row r="594" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A594" s="2" t="s">
         <v>116</v>
       </c>
@@ -22162,7 +22161,7 @@
       <c r="K594" s="2"/>
       <c r="L594" s="2"/>
     </row>
-    <row r="595" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A595" s="2" t="s">
         <v>116</v>
       </c>
@@ -22194,7 +22193,7 @@
       <c r="K595" s="2"/>
       <c r="L595" s="2"/>
     </row>
-    <row r="596" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A596" s="2" t="s">
         <v>116</v>
       </c>
@@ -22226,7 +22225,7 @@
       <c r="K596" s="2"/>
       <c r="L596" s="2"/>
     </row>
-    <row r="597" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A597" s="2" t="s">
         <v>116</v>
       </c>
@@ -22326,7 +22325,7 @@
       </c>
       <c r="L599" s="2"/>
     </row>
-    <row r="600" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A600" s="2" t="s">
         <v>116</v>
       </c>
@@ -22356,7 +22355,7 @@
       <c r="K600" s="2"/>
       <c r="L600" s="2"/>
     </row>
-    <row r="601" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A601" s="2" t="s">
         <v>152</v>
       </c>
@@ -22386,7 +22385,7 @@
       <c r="K601" s="2"/>
       <c r="L601" s="2"/>
     </row>
-    <row r="602" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A602" s="2" t="s">
         <v>152</v>
       </c>
@@ -22416,7 +22415,7 @@
       <c r="K602" s="2"/>
       <c r="L602" s="2"/>
     </row>
-    <row r="603" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A603" s="2" t="s">
         <v>116</v>
       </c>
@@ -22446,7 +22445,7 @@
       <c r="K603" s="2"/>
       <c r="L603" s="2"/>
     </row>
-    <row r="604" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A604" s="2" t="s">
         <v>116</v>
       </c>
@@ -22476,7 +22475,7 @@
       <c r="K604" s="2"/>
       <c r="L604" s="2"/>
     </row>
-    <row r="605" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A605" s="2" t="s">
         <v>152</v>
       </c>
@@ -22506,7 +22505,7 @@
       <c r="K605" s="2"/>
       <c r="L605" s="2"/>
     </row>
-    <row r="606" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A606" s="2" t="s">
         <v>152</v>
       </c>
@@ -22536,7 +22535,7 @@
       <c r="K606" s="2"/>
       <c r="L606" s="2"/>
     </row>
-    <row r="607" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A607" s="2" t="s">
         <v>152</v>
       </c>
@@ -22566,7 +22565,7 @@
       <c r="K607" s="2"/>
       <c r="L607" s="2"/>
     </row>
-    <row r="608" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A608" s="2" t="s">
         <v>152</v>
       </c>
@@ -22632,7 +22631,7 @@
       </c>
       <c r="L609" s="2"/>
     </row>
-    <row r="610" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A610" s="2" t="s">
         <v>152</v>
       </c>
@@ -22662,7 +22661,7 @@
       <c r="K610" s="2"/>
       <c r="L610" s="2"/>
     </row>
-    <row r="611" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A611" s="2" t="s">
         <v>152</v>
       </c>
@@ -22692,7 +22691,7 @@
       <c r="K611" s="2"/>
       <c r="L611" s="2"/>
     </row>
-    <row r="612" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612" s="2" t="s">
         <v>152</v>
       </c>
@@ -22722,7 +22721,7 @@
       <c r="K612" s="2"/>
       <c r="L612" s="2"/>
     </row>
-    <row r="613" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A613" s="2" t="s">
         <v>152</v>
       </c>
@@ -22824,7 +22823,7 @@
       </c>
       <c r="L615" s="2"/>
     </row>
-    <row r="616" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A616" s="2" t="s">
         <v>152</v>
       </c>
@@ -22856,7 +22855,7 @@
       <c r="K616" s="2"/>
       <c r="L616" s="2"/>
     </row>
-    <row r="617" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A617" s="2" t="s">
         <v>152</v>
       </c>
@@ -22922,7 +22921,7 @@
       </c>
       <c r="L618" s="2"/>
     </row>
-    <row r="619" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619" s="2" t="s">
         <v>152</v>
       </c>
@@ -22950,7 +22949,7 @@
       <c r="K619" s="2"/>
       <c r="L619" s="2"/>
     </row>
-    <row r="620" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620" s="2" t="s">
         <v>152</v>
       </c>
@@ -22980,7 +22979,7 @@
       <c r="K620" s="2"/>
       <c r="L620" s="2"/>
     </row>
-    <row r="621" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A621" s="2" t="s">
         <v>152</v>
       </c>
@@ -23010,7 +23009,7 @@
       <c r="K621" s="2"/>
       <c r="L621" s="2"/>
     </row>
-    <row r="622" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A622" s="2" t="s">
         <v>343</v>
       </c>
@@ -23112,7 +23111,7 @@
       </c>
       <c r="L624" s="2"/>
     </row>
-    <row r="625" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A625" s="2" t="s">
         <v>343</v>
       </c>
@@ -23142,7 +23141,7 @@
       <c r="K625" s="2"/>
       <c r="L625" s="2"/>
     </row>
-    <row r="626" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A626" s="2" t="s">
         <v>345</v>
       </c>
@@ -23172,7 +23171,7 @@
       <c r="K626" s="2"/>
       <c r="L626" s="2"/>
     </row>
-    <row r="627" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A627" s="2" t="s">
         <v>345</v>
       </c>
@@ -23276,7 +23275,7 @@
       </c>
       <c r="L629" s="2"/>
     </row>
-    <row r="630" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A630" s="2" t="s">
         <v>345</v>
       </c>
@@ -23306,7 +23305,7 @@
       <c r="K630" s="2"/>
       <c r="L630" s="2"/>
     </row>
-    <row r="631" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="631" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A631" s="2" t="s">
         <v>345</v>
       </c>
@@ -23338,7 +23337,7 @@
       <c r="K631" s="2"/>
       <c r="L631" s="2"/>
     </row>
-    <row r="632" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="632" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A632" s="2" t="s">
         <v>345</v>
       </c>
@@ -23406,7 +23405,7 @@
       </c>
       <c r="L633" s="2"/>
     </row>
-    <row r="634" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A634" s="2" t="s">
         <v>345</v>
       </c>
@@ -23438,7 +23437,7 @@
       <c r="K634" s="2"/>
       <c r="L634" s="2"/>
     </row>
-    <row r="635" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A635" s="2" t="s">
         <v>345</v>
       </c>
@@ -23470,7 +23469,7 @@
       <c r="K635" s="2"/>
       <c r="L635" s="2"/>
     </row>
-    <row r="636" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A636" s="2" t="s">
         <v>345</v>
       </c>
@@ -23572,7 +23571,7 @@
       </c>
       <c r="L638" s="2"/>
     </row>
-    <row r="639" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A639" s="2" t="s">
         <v>345</v>
       </c>
@@ -23676,7 +23675,7 @@
       </c>
       <c r="L641" s="2"/>
     </row>
-    <row r="642" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A642" s="2" t="s">
         <v>345</v>
       </c>
@@ -23780,7 +23779,7 @@
       </c>
       <c r="L644" s="2"/>
     </row>
-    <row r="645" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A645" s="2" t="s">
         <v>345</v>
       </c>
@@ -23812,7 +23811,7 @@
       <c r="K645" s="2"/>
       <c r="L645" s="2"/>
     </row>
-    <row r="646" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A646" s="2" t="s">
         <v>103</v>
       </c>
@@ -23842,7 +23841,7 @@
       <c r="K646" s="2"/>
       <c r="L646" s="2"/>
     </row>
-    <row r="647" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A647" s="2" t="s">
         <v>103</v>
       </c>
@@ -23872,7 +23871,7 @@
       <c r="K647" s="2"/>
       <c r="L647" s="2"/>
     </row>
-    <row r="648" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A648" s="2" t="s">
         <v>746</v>
       </c>
@@ -23903,7 +23902,13 @@
       <c r="L648" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L648" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L648" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Entrega Exitosa"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>